<commit_message>
updates to master_file.ipynb to not have lists of the dataframes as updates weren't being applied correctly.
</commit_message>
<xml_diff>
--- a/data/MarijuanaApplicants - test data list 1.xlsx
+++ b/data/MarijuanaApplicants - test data list 1.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Retailers 11-07" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Retailers 11-07'!$A$1:$L$746</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Retailers 11-07'!$A$1:$K$746</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -5180,7 +5180,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15997,7 +15997,7 @@
       <c r="D807" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L746"/>
+  <autoFilter ref="A1:K746"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>